<commit_message>
Updates CAEX 2.15 metamodel due to inconsistency
Set multiplicity of reference RoleRequirements.roleClass to [0..1]
(instead of [1..1]) in correspondence with the attribute
RoleRequirements.refBaseRoleClassPath [0..1]
</commit_message>
<xml_diff>
--- a/documentation/CAEX30/ChangeDocumentation.xlsx
+++ b/documentation/CAEX30/ChangeDocumentation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="149">
   <si>
     <t>High-Level Change</t>
   </si>
@@ -461,6 +461,9 @@
   </si>
   <si>
     <t>Update of schema version from 2.15 to 3.00</t>
+  </si>
+  <si>
+    <t>RoleRequirements.roleClass (from 0 to 1)</t>
   </si>
 </sst>
 </file>
@@ -794,7 +797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -863,18 +866,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -889,6 +880,21 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1195,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,16 +1222,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1260,13 +1266,13 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="48" t="s">
         <v>113</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -1290,9 +1296,9 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="10" t="s">
         <v>8</v>
       </c>
@@ -1314,9 +1320,9 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="9" t="s">
         <v>9</v>
       </c>
@@ -1369,14 +1375,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="48" t="s">
         <v>50</v>
       </c>
       <c r="D7" s="9" t="s">
@@ -1400,29 +1406,21 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>55</v>
-      </c>
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="9" t="s">
         <v>74</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="I8" s="28"/>
       <c r="J8" s="28" t="s">
@@ -1430,17 +1428,23 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
+      <c r="A9" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>54</v>
+      </c>
       <c r="D9" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>74</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>45</v>
@@ -1454,33 +1458,33 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="25"/>
+      <c r="A10" s="48"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="E10" s="9" t="s">
         <v>74</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>131</v>
-      </c>
+      <c r="H10" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10" s="28"/>
       <c r="J10" s="28" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
       <c r="D11" s="25"/>
       <c r="E11" s="9" t="s">
         <v>74</v>
@@ -1502,47 +1506,47 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="48"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="J12" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B13" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C13" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>45</v>
@@ -1556,17 +1560,17 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
       <c r="D14" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>73</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>45</v>
@@ -1580,15 +1584,17 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="25"/>
+      <c r="A15" s="48"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="E15" s="9" t="s">
         <v>73</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>45</v>
@@ -1602,25 +1608,21 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="40" t="s">
-        <v>115</v>
-      </c>
+      <c r="A16" s="48"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="25"/>
-      <c r="E16" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>85</v>
+      <c r="E16" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="I16" s="28"/>
       <c r="J16" s="28" t="s">
@@ -1628,15 +1630,19 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>115</v>
+      </c>
       <c r="D17" s="25"/>
       <c r="E17" s="10" t="s">
         <v>65</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>45</v>
@@ -1650,15 +1656,15 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
       <c r="D18" s="25"/>
       <c r="E18" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>143</v>
+        <v>86</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>45</v>
@@ -1672,72 +1678,68 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="25"/>
       <c r="E19" s="10" t="s">
         <v>66</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I19" s="28"/>
       <c r="J19" s="28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>119</v>
-      </c>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="49"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
       <c r="D20" s="25"/>
       <c r="E20" s="10" t="s">
         <v>66</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I20" s="28"/>
       <c r="J20" s="28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="C21" s="40" t="s">
-        <v>121</v>
+    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>45</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="I21" s="28"/>
       <c r="J21" s="28" t="s">
@@ -1745,15 +1747,19 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
+      <c r="A22" s="48"/>
+      <c r="B22" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>121</v>
+      </c>
       <c r="D22" s="25"/>
-      <c r="E22" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>142</v>
+      <c r="E22" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>45</v>
@@ -1767,70 +1773,69 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="A23" s="48"/>
+      <c r="B23" s="48"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>146</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="10" t="s">
+      <c r="D24" s="25"/>
+      <c r="E24" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F24" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="7" t="s">
+      <c r="G24" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="J23" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="F24" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H24" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="I24" s="47" t="s">
-        <v>138</v>
-      </c>
-      <c r="J24" t="s">
-        <v>139</v>
+      <c r="J24" s="28" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="25"/>
-      <c r="E25" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="G25" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="I25" s="47" t="s">
-        <v>136</v>
+      <c r="E25" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="G25" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="I25" s="43" t="s">
+        <v>138</v>
       </c>
       <c r="J25" t="s">
         <v>139</v>
@@ -1840,20 +1845,20 @@
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="25"/>
-      <c r="E26" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="F26" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="G26" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H26" s="46" t="s">
+      <c r="E26" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="H26" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="47" t="s">
-        <v>135</v>
+      <c r="I26" s="43" t="s">
+        <v>136</v>
       </c>
       <c r="J26" t="s">
         <v>139</v>
@@ -1863,19 +1868,19 @@
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="25"/>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="F27" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="G27" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" s="46" t="s">
+      <c r="F27" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="47" t="s">
+      <c r="I27" s="43" t="s">
         <v>135</v>
       </c>
       <c r="J27" t="s">
@@ -1886,20 +1891,20 @@
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="25"/>
-      <c r="E28" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="G28" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H28" s="46" t="s">
-        <v>129</v>
-      </c>
-      <c r="I28" s="47" t="s">
-        <v>134</v>
+      <c r="E28" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" s="43" t="s">
+        <v>135</v>
       </c>
       <c r="J28" t="s">
         <v>139</v>
@@ -1909,19 +1914,19 @@
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="25"/>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="F29" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="G29" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H29" s="46" t="s">
+      <c r="F29" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="I29" s="47" t="s">
+      <c r="I29" s="43" t="s">
         <v>134</v>
       </c>
       <c r="J29" t="s">
@@ -1932,20 +1937,20 @@
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="25"/>
-      <c r="E30" s="49" t="s">
-        <v>67</v>
-      </c>
-      <c r="F30" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="G30" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H30" s="46" t="s">
+      <c r="E30" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="G30" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="I30" s="47" t="s">
-        <v>133</v>
+      <c r="I30" s="43" t="s">
+        <v>134</v>
       </c>
       <c r="J30" t="s">
         <v>139</v>
@@ -1955,20 +1960,20 @@
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="25"/>
-      <c r="E31" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="F31" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="G31" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H31" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" s="47" t="s">
-        <v>132</v>
+      <c r="E31" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="I31" s="43" t="s">
+        <v>133</v>
       </c>
       <c r="J31" t="s">
         <v>139</v>
@@ -1978,19 +1983,19 @@
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="25"/>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="G32" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H32" s="46" t="s">
+      <c r="F32" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="G32" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="47" t="s">
+      <c r="I32" s="43" t="s">
         <v>132</v>
       </c>
       <c r="J32" t="s">
@@ -2001,19 +2006,19 @@
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="25"/>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="F33" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="G33" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H33" s="46" t="s">
+      <c r="F33" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H33" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="47" t="s">
+      <c r="I33" s="43" t="s">
         <v>132</v>
       </c>
       <c r="J33" t="s">
@@ -2024,19 +2029,19 @@
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="25"/>
-      <c r="E34" s="49" t="s">
+      <c r="E34" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="F34" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="G34" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H34" s="46" t="s">
+      <c r="F34" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="G34" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="I34" s="28" t="s">
+      <c r="I34" s="43" t="s">
         <v>132</v>
       </c>
       <c r="J34" t="s">
@@ -2046,20 +2051,20 @@
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="44"/>
-      <c r="E35" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="F35" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="H35" s="46" t="s">
+      <c r="D35" s="25"/>
+      <c r="E35" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="G35" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="I35" s="47" t="s">
+      <c r="I35" s="28" t="s">
         <v>132</v>
       </c>
       <c r="J35" t="s">
@@ -2067,8 +2072,27 @@
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="G36" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="H36" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="J36" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
@@ -2094,25 +2118,32 @@
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="20">
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
     <mergeCell ref="D1:F1"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="A9:A12"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates change documentation sheet
</commit_message>
<xml_diff>
--- a/documentation/CAEX30/ChangeDocumentation.xlsx
+++ b/documentation/CAEX30/ChangeDocumentation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="143">
   <si>
     <t>High-Level Change</t>
   </si>
@@ -285,58 +285,13 @@
     <t>Mapping.interfaceNameMapping (renamed to interfaceIDMapping)</t>
   </si>
   <si>
-    <t>ExternalInterface.externalInterface</t>
-  </si>
-  <si>
-    <t>InternalLink.partnerSideA (type changed from InterfaceClass to ExternalInterface)</t>
-  </si>
-  <si>
-    <t>InternalLink.partnerSideB (type changed from InterfaceClass to ExternalInterface)</t>
-  </si>
-  <si>
     <t>InternalLink.partnerSideA (from 0 to 1)</t>
   </si>
   <si>
     <t>(NB) Property.lowerBound - Decrease</t>
   </si>
   <si>
-    <t>Reflected in Metamodels</t>
-  </si>
-  <si>
-    <t>Reflected in Images</t>
-  </si>
-  <si>
-    <t>OrdinalSclaed (renamed to OrdinalScaledType)</t>
-  </si>
-  <si>
-    <t>NominalScaled (renamed to NominalScaledType)</t>
-  </si>
-  <si>
-    <t>NominalScaled.requiredValue (from 1 to *)</t>
-  </si>
-  <si>
-    <t>ExternalReference (renamed to ExternalReferenceType)</t>
-  </si>
-  <si>
     <t>CAEXFile.schemaVersion (default value set from "2.15" to "3.00")</t>
-  </si>
-  <si>
-    <t>CAEXBasicObject.description</t>
-  </si>
-  <si>
-    <t>CAEXBasicObject.version</t>
-  </si>
-  <si>
-    <t>CAEXBasicObject.revision</t>
-  </si>
-  <si>
-    <t>CAEXBasicObject.copyright</t>
-  </si>
-  <si>
-    <t>CAEXBasicObject.additionalInformation (from * to 1)</t>
-  </si>
-  <si>
-    <t>Documented in slides from Rainer</t>
   </si>
   <si>
     <t>Mandatory role class assignment for role requirements</t>
@@ -367,9 +322,6 @@
     <t>Introduction of support for attribute libraries</t>
   </si>
   <si>
-    <t>slide 28; what is actually introduced there is a containment InterfaceClass.externalInterface : Interface; but it is missing in the metamodel</t>
-  </si>
-  <si>
     <t>slide 33</t>
   </si>
   <si>
@@ -394,51 +346,12 @@
     <t>slide 69</t>
   </si>
   <si>
-    <t>(NB) Property.defaultValue - Update</t>
-  </si>
-  <si>
     <t>Change default value of property</t>
   </si>
   <si>
-    <t>no, see slide 33</t>
-  </si>
-  <si>
     <t>slide 35 (example)</t>
   </si>
   <si>
-    <t>no, see slide 23</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>should be ok</t>
-  </si>
-  <si>
-    <t>changed back</t>
-  </si>
-  <si>
-    <t>changed to 0..* in CAEX 2.15 and CAEX 3.0</t>
-  </si>
-  <si>
-    <t>should be the same in both versions, removed "Type" appendix in CAEX 3.0</t>
-  </si>
-  <si>
-    <t>should be InterfaceClass in both versions; changed to InterfaceClass in Version 3.0</t>
-  </si>
-  <si>
-    <t>should be a containment owned by InterfaceClass (introduced in CAEX 3.0), changed in CAEX version 3.0</t>
-  </si>
-  <si>
-    <t>change applied for CAEX 3.0</t>
-  </si>
-  <si>
-    <t>changed name back to ExternalReference in CAEX 3.0</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Attribute.refAttributeType : String</t>
   </si>
   <si>
@@ -464,23 +377,85 @@
   </si>
   <si>
     <t>RoleRequirements.roleClass (from 0 to 1)</t>
+  </si>
+  <si>
+    <t>InternalLink.partnerSideB (from 0 to 1)</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>Documentation in CAEX Maintenance Cycle Presentation</t>
+  </si>
+  <si>
+    <t>slide 28</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>Attribute.referenceAttribute : Attribute</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>H8</t>
+  </si>
+  <si>
+    <t>H9</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>BC10</t>
+  </si>
+  <si>
+    <t>(B) Property.defaultValue - Update</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -513,57 +488,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="6"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -797,19 +728,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -818,71 +752,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -891,12 +786,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1201,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,25 +1122,22 @@
     <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="80.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.5703125" style="37" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" style="7" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -1252,55 +1156,39 @@
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="I2" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="G2" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="B3" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="29" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>66</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="10" t="s">
-        <v>8</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29" t="s">
+        <v>7</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>67</v>
@@ -1309,22 +1197,15 @@
         <v>63</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="9" t="s">
-        <v>9</v>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="30" t="s">
+        <v>8</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>70</v>
@@ -1333,18 +1214,11 @@
         <v>64</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
         <v>46</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -1353,194 +1227,139 @@
       <c r="C6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>7</v>
+      <c r="D6" s="29" t="s">
+        <v>9</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>66</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="J6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="G6" s="23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="48" t="s">
+      <c r="B7" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>51</v>
+      <c r="D7" s="30" t="s">
+        <v>60</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>74</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="50"/>
+        <v>119</v>
+      </c>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="30" t="s">
+        <v>137</v>
+      </c>
       <c r="E8" s="9" t="s">
         <v>74</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>148</v>
+        <v>79</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>55</v>
+      <c r="D9" s="30" t="s">
+        <v>61</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>74</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="9" t="s">
-        <v>56</v>
+        <v>89</v>
+      </c>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="30" t="s">
+        <v>62</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>74</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="25"/>
+        <v>120</v>
+      </c>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="30" t="s">
+        <v>138</v>
+      </c>
       <c r="E11" s="9" t="s">
         <v>74</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="J11" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="25"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="30" t="s">
+        <v>139</v>
+      </c>
       <c r="E12" s="9" t="s">
         <v>74</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="J12" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>60</v>
+      <c r="D13" s="30" t="s">
+        <v>51</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>72</v>
@@ -1548,96 +1367,72 @@
       <c r="F13" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="G13" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="9" t="s">
-        <v>61</v>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="30" t="s">
+        <v>55</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>73</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="9" t="s">
-        <v>62</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="30" t="s">
+        <v>56</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>73</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="25"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="30" t="s">
+        <v>121</v>
+      </c>
       <c r="E16" s="9" t="s">
         <v>73</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="49"/>
-      <c r="B17" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17" s="48" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17" s="25"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>122</v>
+      </c>
       <c r="E17" s="10" t="s">
         <v>65</v>
       </c>
@@ -1645,499 +1440,205 @@
         <v>85</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="49"/>
-      <c r="B18" s="48"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="25"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29" t="s">
+        <v>123</v>
+      </c>
       <c r="E18" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>143</v>
-      </c>
       <c r="G19" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="49"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="25"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="29" t="s">
+        <v>131</v>
+      </c>
       <c r="E20" s="10" t="s">
         <v>66</v>
       </c>
       <c r="F20" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D21" s="25"/>
       <c r="E21" s="10" t="s">
         <v>66</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H21" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="48" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="48"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="9" t="s">
+      <c r="C25" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>128</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>146</v>
-      </c>
-      <c r="C24" t="s">
-        <v>147</v>
-      </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="J24" s="28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="G25" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" s="42" t="s">
-        <v>127</v>
-      </c>
-      <c r="I25" s="43" t="s">
-        <v>138</v>
-      </c>
-      <c r="J25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="G26" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="H26" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="I26" s="43" t="s">
-        <v>136</v>
-      </c>
-      <c r="J26" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="G27" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="I27" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="J27" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="44" t="s">
-        <v>76</v>
-      </c>
-      <c r="F28" s="44" t="s">
+      <c r="F25" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="G28" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H28" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="I28" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="J28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="G29" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H29" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="I29" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="J29" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="G30" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H30" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="I30" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="J30" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="F31" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="G31" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H31" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="I31" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="J31" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H32" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="I32" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="J32" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="F33" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="G33" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H33" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="I33" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="J33" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="G34" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H34" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="I34" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="J34" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="F35" s="45" t="s">
-        <v>104</v>
-      </c>
-      <c r="G35" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H35" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="I35" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="J35" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="F36" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="G36" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="H36" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="J36" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="G25" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="A17:A21"/>
     <mergeCell ref="C3:C5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
     <mergeCell ref="D1:F1"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="A13:A16"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="A17:A20"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="A9:A12"/>
@@ -2167,7 +1668,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,16 +1693,16 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="39" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2224,7 +1725,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>16</v>
@@ -2261,55 +1762,57 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>13</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="32" t="s">
+      <c r="A9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>45</v>
@@ -2317,13 +1820,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>45</v>
@@ -2331,13 +1834,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>45</v>
@@ -2345,13 +1848,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>45</v>
@@ -2359,13 +1862,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>45</v>
@@ -2373,13 +1876,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>45</v>
@@ -2387,29 +1890,29 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="22" t="s">
+      <c r="A17" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates CAEX 3.0 change documentation
</commit_message>
<xml_diff>
--- a/documentation/CAEX30/ChangeDocumentation.xlsx
+++ b/documentation/CAEX30/ChangeDocumentation.xlsx
@@ -179,10 +179,6 @@
     <t>Mandatory linking of internal links</t>
   </si>
   <si>
-    <t xml:space="preserve"> Prescription of mandatory linking of external interfaces
-via internal links</t>
-  </si>
-  <si>
     <t>C9</t>
   </si>
   <si>
@@ -289,9 +285,6 @@
   </si>
   <si>
     <t>(NB) Property.lowerBound - Decrease</t>
-  </si>
-  <si>
-    <t>CAEXFile.schemaVersion (default value set from "2.15" to "3.00")</t>
   </si>
   <si>
     <t>Mandatory role class assignment for role requirements</t>
@@ -328,15 +321,9 @@
     <t>Superior standard version information</t>
   </si>
   <si>
-    <t>Introduction of support to store version information of a superior standard, e.g., "AutomationML 2.0"</t>
-  </si>
-  <si>
     <t>Data source</t>
   </si>
   <si>
-    <t>Introduction of support for naming data source (=source tool)</t>
-  </si>
-  <si>
     <t>slide 38</t>
   </si>
   <si>
@@ -446,6 +433,18 @@
   </si>
   <si>
     <t>(B) Property.defaultValue - Update</t>
+  </si>
+  <si>
+    <t>CAEXFile.schemaVersion (from "2.15" to "3.00")</t>
+  </si>
+  <si>
+    <t>Prescription of mandatory linking of external interfaces via internal links</t>
+  </si>
+  <si>
+    <t>Introduction of support to store version information of superior standards, e.g., "AutomationML 2.0"</t>
+  </si>
+  <si>
+    <t>Introduction of support to store data source (=source tool)</t>
   </si>
 </sst>
 </file>
@@ -497,7 +496,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -724,11 +723,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -738,22 +827,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -771,31 +848,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -804,6 +857,94 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1111,7 +1252,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,477 +1263,477 @@
     <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="80.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" style="7" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" style="6" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="E1" s="54"/>
+      <c r="F1" s="55"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="40"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="19"/>
+    </row>
+    <row r="8" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="40"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="40"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="40"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="40"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="40" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="28" t="s">
+      <c r="B17" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C17" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="D17" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="40"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G4" s="8" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="9" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="40"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="40"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="E24" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G7" s="23"/>
-    </row>
-    <row r="8" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="30" t="s">
-        <v>137</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="30" t="s">
+      <c r="F24" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="50" t="s">
         <v>138</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="30" t="s">
+      <c r="F25" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" s="8" t="s">
+      <c r="G25" s="6" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1625,13 +1766,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C17:C21"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
@@ -1645,6 +1779,13 @@
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1693,226 +1834,226 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="39" t="s">
+      <c r="C3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="13" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="14" t="s">
+      <c r="C5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="14" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="14" t="s">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="15" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="36" t="s">
+      <c r="C9" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="18" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="19" t="s">
+      <c r="C10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="18" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="19" t="s">
+      <c r="C11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="18" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="19" t="s">
+      <c r="C12" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="18" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="19" t="s">
+      <c r="C13" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="18" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C13" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="19" t="s">
+      <c r="C14" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="18" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="19" t="s">
+      <c r="C15" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="18" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="19" t="s">
+      <c r="C16" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="D17" s="21" t="s">
+      <c r="A17" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>